<commit_message>
removing wrong samplesheets for rnaseq - remake these after fetchNGS is done
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Resilience_Biomarkers_Aquaculture\Cvirg_Pmarinus_RNAseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699B136A-4E46-44B3-8C8D-045F461BB2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30318430-0674-4F4F-871E-91307848B335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,13 +216,13 @@
     <t>Set #</t>
   </si>
   <si>
-    <t>SRX765s</t>
-  </si>
-  <si>
     <t>SRX564s</t>
   </si>
   <si>
     <t>SRX984s</t>
+  </si>
+  <si>
+    <t>SRX7656s</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +757,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>27</v>
@@ -797,7 +797,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>32</v>
@@ -837,7 +837,7 @@
         <v>36</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
changing samplesheet R script and metadata spreadsheet
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Resilience_Biomarkers_Aquaculture\Cvirg_Pmarinus_RNAseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30318430-0674-4F4F-871E-91307848B335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F66F1F-316A-48B0-AA1C-7CE823796847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Species</t>
   </si>
@@ -61,9 +72,6 @@
   </si>
   <si>
     <t>DEG data</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>resilience</t>
@@ -114,9 +122,6 @@
     <t>https://www.ncbi.nlm.nih.gov/sra?LinkName=bioproject_sra_all&amp;from_uid=894694</t>
   </si>
   <si>
-    <t>E,T</t>
-  </si>
-  <si>
     <t>infected</t>
   </si>
   <si>
@@ -156,9 +161,6 @@
     <t>SraRunTable(1).csv</t>
   </si>
   <si>
-    <t>C. gigas &amp; virginica</t>
-  </si>
-  <si>
     <r>
       <t>Chan </t>
     </r>
@@ -216,20 +218,47 @@
     <t>Set #</t>
   </si>
   <si>
-    <t>SRX564s</t>
-  </si>
-  <si>
     <t>SRX984s</t>
   </si>
   <si>
     <t>SRX7656s</t>
+  </si>
+  <si>
+    <t>Tissue type</t>
+  </si>
+  <si>
+    <t>Mantle</t>
+  </si>
+  <si>
+    <t>Number of samples</t>
+  </si>
+  <si>
+    <t>Number of files</t>
+  </si>
+  <si>
+    <t>RNAseq</t>
+  </si>
+  <si>
+    <t>TAGseq</t>
+  </si>
+  <si>
+    <t>Gill</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>This study also had pacific oyster but not included in this meta table</t>
+  </si>
+  <si>
+    <t>SRX130s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,13 +295,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,7 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -331,23 +379,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -630,240 +681,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="8" width="15.77734375" customWidth="1"/>
-    <col min="9" max="10" width="23.21875" customWidth="1"/>
-    <col min="11" max="11" width="37.88671875" customWidth="1"/>
-    <col min="12" max="14" width="15.77734375" customWidth="1"/>
+    <col min="2" max="9" width="15.77734375" customWidth="1"/>
+    <col min="10" max="13" width="23.21875" customWidth="1"/>
+    <col min="14" max="14" width="37.88671875" customWidth="1"/>
+    <col min="15" max="17" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+    <row r="2" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7">
+        <v>61</v>
+      </c>
+      <c r="L2" s="7">
+        <f>K2*2</f>
+        <v>122</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="9">
+        <v>40</v>
+      </c>
+      <c r="L3" s="9">
+        <v>40</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="H4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="J4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="K4" s="7">
+        <v>10</v>
+      </c>
+      <c r="L4" s="7">
+        <v>10</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="9">
+        <v>44</v>
+      </c>
+      <c r="L5" s="9">
+        <f>K5*2</f>
+        <v>88</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="O5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="10">
+        <f>SUM(K2:K5)</f>
+        <v>155</v>
+      </c>
+      <c r="L8" s="10">
+        <f>SUM(L2:L5)</f>
+        <v>260</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{45A84F04-539F-4EA4-9869-B11B92C6202C}"/>
-    <hyperlink ref="K2" r:id="rId2" xr:uid="{A296B386-A9E9-426B-9889-2B0BBCA5D2A7}"/>
-    <hyperlink ref="L2" r:id="rId3" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable.csv" xr:uid="{2A9959DB-24F8-4CF5-9430-AAE23C4D28EA}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{93530DC1-A712-4B93-96B1-5D1B9EA1D58D}"/>
-    <hyperlink ref="K3" r:id="rId5" xr:uid="{BF5990C2-05A4-4B84-8D44-FFBF5701F285}"/>
-    <hyperlink ref="L3" r:id="rId6" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (1).csv" xr:uid="{2DC83621-507F-4ABA-9B19-28C64B64B168}"/>
-    <hyperlink ref="I4" r:id="rId7" display="https://resilience-biomarkers-for-aquaculture.github.io/about/10.3389/fgene.2021.795706" xr:uid="{9E90EDBF-5FCF-44FE-8180-B25247D41E8E}"/>
-    <hyperlink ref="K4" r:id="rId8" xr:uid="{9213CC98-A144-4B01-AC64-22E94B102CA4}"/>
-    <hyperlink ref="L4" r:id="rId9" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (2).csv" xr:uid="{7AE54867-BA31-4C78-B186-3DD1D11AD0FD}"/>
-    <hyperlink ref="I5" r:id="rId10" xr:uid="{35E594CD-02BC-4B88-BAF4-91707E113446}"/>
-    <hyperlink ref="K5" r:id="rId11" xr:uid="{CBC05E43-ABE2-4904-B565-91A48713CEAE}"/>
-    <hyperlink ref="L5" r:id="rId12" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (3).csv" xr:uid="{44C068B3-9B15-466D-BD11-F8FA066910FB}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{45A84F04-539F-4EA4-9869-B11B92C6202C}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{A296B386-A9E9-426B-9889-2B0BBCA5D2A7}"/>
+    <hyperlink ref="O2" r:id="rId3" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable.csv" xr:uid="{2A9959DB-24F8-4CF5-9430-AAE23C4D28EA}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{93530DC1-A712-4B93-96B1-5D1B9EA1D58D}"/>
+    <hyperlink ref="N3" r:id="rId5" xr:uid="{BF5990C2-05A4-4B84-8D44-FFBF5701F285}"/>
+    <hyperlink ref="O3" r:id="rId6" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (1).csv" xr:uid="{2DC83621-507F-4ABA-9B19-28C64B64B168}"/>
+    <hyperlink ref="O4" r:id="rId7" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (2).csv" xr:uid="{7AE54867-BA31-4C78-B186-3DD1D11AD0FD}"/>
+    <hyperlink ref="J5" r:id="rId8" xr:uid="{35E594CD-02BC-4B88-BAF4-91707E113446}"/>
+    <hyperlink ref="N5" r:id="rId9" xr:uid="{CBC05E43-ABE2-4904-B565-91A48713CEAE}"/>
+    <hyperlink ref="O5" r:id="rId10" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (3).csv" xr:uid="{44C068B3-9B15-466D-BD11-F8FA066910FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
additions to metadata table
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Resilience_Biomarkers_Aquaculture\Cvirg_Pmarinus_RNAseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F66F1F-316A-48B0-AA1C-7CE823796847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE5C29-7DBD-4805-988D-69EC355133E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Species</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>SRX130s</t>
+  </si>
+  <si>
+    <t>Ran dataset 3</t>
+  </si>
+  <si>
+    <t>Index of /emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset3</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -400,6 +406,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -681,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,6 +970,17 @@
         <v>260</v>
       </c>
     </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="11">
+        <v>45632</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{45A84F04-539F-4EA4-9869-B11B92C6202C}"/>
@@ -974,8 +993,9 @@
     <hyperlink ref="J5" r:id="rId8" xr:uid="{35E594CD-02BC-4B88-BAF4-91707E113446}"/>
     <hyperlink ref="N5" r:id="rId9" xr:uid="{CBC05E43-ABE2-4904-B565-91A48713CEAE}"/>
     <hyperlink ref="O5" r:id="rId10" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (3).csv" xr:uid="{44C068B3-9B15-466D-BD11-F8FA066910FB}"/>
+    <hyperlink ref="D12" r:id="rId11" display="https://gannet.fish.washington.edu/emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset3/" xr:uid="{5079A8C0-7971-4F57-9260-6C82B24A9CBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edits to metadata infomation
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Resilience_Biomarkers_Aquaculture\Cvirg_Pmarinus_RNAseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE5C29-7DBD-4805-988D-69EC355133E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1853C47D-029A-47C0-B6CA-5DBFBB947285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Species</t>
   </si>
@@ -258,6 +258,33 @@
   </si>
   <si>
     <t>Index of /emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset3</t>
+  </si>
+  <si>
+    <t>Ran dataset 2</t>
+  </si>
+  <si>
+    <t>Index of /emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset2</t>
+  </si>
+  <si>
+    <t>Ran dataset 4</t>
+  </si>
+  <si>
+    <t>Index of /emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset4</t>
+  </si>
+  <si>
+    <t>Run dataset 1</t>
+  </si>
+  <si>
+    <t>Index of /emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset1</t>
+  </si>
+  <si>
+    <t>Cgigas dataset 3</t>
+  </si>
+  <si>
+    <t>running..</t>
+  </si>
+  <si>
+    <t>C. virginica / C.gigas</t>
   </si>
 </sst>
 </file>
@@ -689,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>47</v>
@@ -979,6 +1006,50 @@
       </c>
       <c r="D12" s="12" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="11">
+        <v>45635</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="11">
+        <v>45635</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="11">
+        <v>45637</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="11">
+        <v>45637</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -994,8 +1065,11 @@
     <hyperlink ref="N5" r:id="rId9" xr:uid="{CBC05E43-ABE2-4904-B565-91A48713CEAE}"/>
     <hyperlink ref="O5" r:id="rId10" display="https://github.com/Resilience-Biomarkers-for-Aquaculture/Cvirg_Pmarinus_RNAseq/blob/main/data/SraRunTable (3).csv" xr:uid="{44C068B3-9B15-466D-BD11-F8FA066910FB}"/>
     <hyperlink ref="D12" r:id="rId11" display="https://gannet.fish.washington.edu/emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset3/" xr:uid="{5079A8C0-7971-4F57-9260-6C82B24A9CBB}"/>
+    <hyperlink ref="D13" r:id="rId12" display="https://gannet.fish.washington.edu/emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset2/" xr:uid="{52EE9229-0AED-4F5E-8DFC-C4A172DC043A}"/>
+    <hyperlink ref="D14" r:id="rId13" display="https://gannet.fish.washington.edu/emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset4/" xr:uid="{EBA5E84D-6B1B-48D3-8FAD-6888BDE329E1}"/>
+    <hyperlink ref="D15" r:id="rId14" display="https://gannet.fish.washington.edu/emma.strand/rnaseq/Cvir_Prkns_rnaseq_dataset1/" xr:uid="{BE32A916-B500-403C-B58F-B9E58ACC6391}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited samplesheet dataset3 and analysis ideas with disease datasets
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Resilience_Biomarkers_Aquaculture\Cvirg_Pmarinus_RNAseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1853C47D-029A-47C0-B6CA-5DBFBB947285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649A513A-5FFD-4594-BBE7-1F554EE77830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Species</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>C. virginica / C.gigas</t>
+  </si>
+  <si>
+    <t>Re-run dataset 3 with different trimming parameters</t>
   </si>
 </sst>
 </file>
@@ -716,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,6 +1053,11 @@
       </c>
       <c r="D16" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>